<commit_message>
add values for unfound results
</commit_message>
<xml_diff>
--- a/results/expressiondata_comparison/brain_expressiondata_comparison.xlsx
+++ b/results/expressiondata_comparison/brain_expressiondata_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s202425/Documents/GitHub/metastasis/results/expressiondata_comparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3872585D-C93B-5C48-B368-809BCF3E2BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8979A57A-9BB1-1746-8DC4-78F0AAA4CF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{4494EFA9-B28A-2643-A177-2F6A16CE7C8C}"/>
+    <workbookView xWindow="5800" yWindow="500" windowWidth="23000" windowHeight="15980" xr2:uid="{4494EFA9-B28A-2643-A177-2F6A16CE7C8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="76">
   <si>
     <t>pathway</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>low</t>
-  </si>
-  <si>
-    <t>not Found</t>
   </si>
   <si>
     <t>HMR_2583</t>
@@ -655,7 +652,7 @@
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -682,7 +679,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -699,7 +696,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>8</v>
@@ -707,11 +704,11 @@
       <c r="E2" s="5">
         <v>9.93</v>
       </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
+      <c r="F2" s="2">
+        <v>-4.268E-16</v>
+      </c>
+      <c r="G2" s="2">
+        <v>3.0820000000000001E-17</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -722,7 +719,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>8</v>
@@ -730,11 +727,11 @@
       <c r="E3" s="5">
         <v>9.93</v>
       </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -742,10 +739,10 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>8</v>
@@ -753,11 +750,11 @@
       <c r="E4" s="5">
         <v>9.93</v>
       </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" t="s">
-        <v>9</v>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -765,10 +762,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>8</v>
@@ -776,11 +773,11 @@
       <c r="E5" s="5">
         <v>9.93</v>
       </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>9</v>
+      <c r="F5" s="2">
+        <v>-1.88304E-12</v>
+      </c>
+      <c r="G5" s="2">
+        <v>-1.3634E-14</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -788,10 +785,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>8</v>
@@ -799,11 +796,11 @@
       <c r="E6" s="5">
         <v>9.93</v>
       </c>
-      <c r="F6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" t="s">
-        <v>9</v>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -811,10 +808,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>8</v>
@@ -822,22 +819,22 @@
       <c r="E7" s="5">
         <v>9.93</v>
       </c>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" t="s">
-        <v>9</v>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
         <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>8</v>
@@ -845,22 +842,22 @@
       <c r="E8" s="6">
         <v>3.65</v>
       </c>
-      <c r="F8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" t="s">
-        <v>9</v>
+      <c r="F8">
+        <v>0.64849999999999997</v>
+      </c>
+      <c r="G8">
+        <v>3.9830999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>8</v>
@@ -877,13 +874,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
         <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>8</v>
@@ -900,13 +897,13 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>8</v>
@@ -921,18 +918,18 @@
         <v>508</v>
       </c>
       <c r="I11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
         <v>28</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>29</v>
-      </c>
-      <c r="C12" t="s">
-        <v>30</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>8</v>
@@ -940,22 +937,22 @@
       <c r="E12" s="1">
         <v>6.4729999999999999</v>
       </c>
-      <c r="F12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" t="s">
-        <v>9</v>
+      <c r="F12" s="2">
+        <v>-9.6799999999999995E-16</v>
+      </c>
+      <c r="G12" s="2">
+        <v>9.8422999999999998E-15</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
         <v>28</v>
       </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>8</v>
@@ -963,22 +960,22 @@
       <c r="E13" s="1">
         <v>6.4729999999999999</v>
       </c>
-      <c r="F13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" t="s">
-        <v>9</v>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
         <v>32</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>33</v>
-      </c>
-      <c r="C14" t="s">
-        <v>34</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>8</v>
@@ -995,13 +992,13 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
         <v>35</v>
-      </c>
-      <c r="C15" t="s">
-        <v>36</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>8</v>
@@ -1009,22 +1006,22 @@
       <c r="E15" s="6">
         <v>3.5430000000000001</v>
       </c>
-      <c r="F15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" t="s">
-        <v>9</v>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
         <v>37</v>
-      </c>
-      <c r="C16" t="s">
-        <v>38</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>8</v>
@@ -1041,13 +1038,13 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>8</v>
@@ -1064,13 +1061,13 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" t="s">
         <v>40</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>41</v>
-      </c>
-      <c r="C18" t="s">
-        <v>42</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>8</v>
@@ -1087,16 +1084,16 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
         <v>43</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>44</v>
       </c>
-      <c r="C19" t="s">
-        <v>45</v>
-      </c>
       <c r="D19" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E19" s="1">
         <v>6.4729999999999999</v>
@@ -1110,16 +1107,16 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20" s="1">
         <v>6.4729999999999999</v>
@@ -1133,16 +1130,16 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E21" s="1">
         <v>6.4729999999999999</v>
@@ -1156,62 +1153,62 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" t="s">
         <v>49</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>50</v>
       </c>
-      <c r="C22" t="s">
-        <v>51</v>
-      </c>
       <c r="D22" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E22" s="1">
         <v>6.0860000000000003</v>
       </c>
-      <c r="F22" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" t="s">
-        <v>9</v>
+      <c r="F22">
+        <v>2.0880000000000001</v>
+      </c>
+      <c r="G22">
+        <v>7.6689999999999996</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" t="s">
         <v>49</v>
       </c>
-      <c r="B23" t="s">
-        <v>50</v>
-      </c>
       <c r="C23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E23" s="1">
         <v>6.0860000000000003</v>
       </c>
-      <c r="F23" t="s">
-        <v>9</v>
-      </c>
-      <c r="G23" t="s">
-        <v>9</v>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" t="s">
         <v>53</v>
       </c>
-      <c r="B24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" t="s">
-        <v>54</v>
-      </c>
       <c r="D24" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E24" s="5">
         <v>9.2439999999999998</v>
@@ -1225,16 +1222,16 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" t="s">
         <v>55</v>
       </c>
-      <c r="B25" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" t="s">
-        <v>56</v>
-      </c>
       <c r="D25" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E25" s="5">
         <v>9.85</v>
@@ -1248,16 +1245,16 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E26" s="5">
         <v>9.85</v>
@@ -1271,16 +1268,16 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E27" s="5">
         <v>9.85</v>
@@ -1294,16 +1291,16 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E28" s="5">
         <v>9.85</v>
@@ -1317,16 +1314,16 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E29" s="5">
         <v>9.85</v>
@@ -1340,16 +1337,16 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E30" s="5">
         <v>9.85</v>
@@ -1363,16 +1360,16 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" t="s">
         <v>33</v>
       </c>
-      <c r="C31" t="s">
-        <v>34</v>
-      </c>
       <c r="D31" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E31" s="6">
         <v>4.17</v>
@@ -1384,21 +1381,21 @@
         <v>0</v>
       </c>
       <c r="I31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
         <v>63</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>64</v>
       </c>
-      <c r="C32" t="s">
-        <v>65</v>
-      </c>
       <c r="D32" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E32" s="6">
         <v>4.17</v>
@@ -1410,21 +1407,21 @@
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E33" s="6">
         <v>4.17</v>
@@ -1436,47 +1433,47 @@
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" t="s">
         <v>35</v>
       </c>
-      <c r="C34" t="s">
-        <v>36</v>
-      </c>
       <c r="D34" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E34" s="6">
         <v>4.17</v>
       </c>
-      <c r="F34" t="s">
-        <v>9</v>
-      </c>
-      <c r="G34" t="s">
-        <v>9</v>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" t="s">
         <v>37</v>
       </c>
-      <c r="C35" t="s">
-        <v>38</v>
-      </c>
       <c r="D35" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E35" s="6">
         <v>4.17</v>
@@ -1488,21 +1485,21 @@
         <v>-5.7867201693752604E-22</v>
       </c>
       <c r="I35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E36" s="6">
         <v>4.17</v>
@@ -1514,21 +1511,21 @@
         <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E37" s="1">
         <v>6.16</v>
@@ -1542,16 +1539,16 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E38" s="1">
         <v>6.16</v>
@@ -1565,94 +1562,94 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" t="s">
         <v>70</v>
       </c>
-      <c r="B39" t="s">
-        <v>29</v>
-      </c>
-      <c r="C39" t="s">
-        <v>71</v>
-      </c>
       <c r="D39" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E39" s="6">
         <v>4.5990000000000002</v>
       </c>
-      <c r="F39" t="s">
-        <v>9</v>
-      </c>
-      <c r="G39" t="s">
-        <v>9</v>
+      <c r="F39">
+        <v>2.8721999999999999</v>
+      </c>
+      <c r="G39">
+        <v>22.842600000000001</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" t="s">
         <v>72</v>
       </c>
-      <c r="B40" t="s">
-        <v>50</v>
-      </c>
-      <c r="C40" t="s">
-        <v>73</v>
-      </c>
       <c r="D40" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E40" s="5">
         <v>8.6590000000000007</v>
       </c>
-      <c r="F40" t="s">
-        <v>9</v>
-      </c>
-      <c r="G40" t="s">
-        <v>9</v>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" t="s">
         <v>50</v>
       </c>
-      <c r="C41" t="s">
-        <v>51</v>
-      </c>
       <c r="D41" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E41" s="7">
         <v>6.79</v>
       </c>
-      <c r="F41" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" t="s">
-        <v>9</v>
+      <c r="F41">
+        <v>2.0886</v>
+      </c>
+      <c r="G41">
+        <v>7.6689999999999996</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E42" s="7">
         <v>6.79</v>
       </c>
-      <c r="F42" t="s">
-        <v>9</v>
-      </c>
-      <c r="G42" t="s">
-        <v>9</v>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>